<commit_message>
Documentation mecmesin list reading
</commit_message>
<xml_diff>
--- a/inst/sampleData/mecmesin/files_stretch.xlsx
+++ b/inst/sampleData/mecmesin/files_stretch.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D235368-46ED-564E-9BB2-26697B2AF91F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A06C644F-1A97-2A46-B01F-DAC9AD726626}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -521,8 +521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="B4" sqref="A4:XFD9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>